<commit_message>
Added tasks which were done during 2-3 weeks
</commit_message>
<xml_diff>
--- a/Weekly Logs.xlsx
+++ b/Weekly Logs.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sunny/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24426"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>• reached out to peers to form group</t>
   </si>
@@ -106,13 +101,25 @@
   </si>
   <si>
     <t>• experiment with Lambda for back-end logic</t>
+  </si>
+  <si>
+    <t>• Worked on UI (SignIn, Teach, Settings)</t>
+  </si>
+  <si>
+    <t>• Worked on the database, fixing errors</t>
+  </si>
+  <si>
+    <t>• Worked on UI (Home, Learn) Created prototypes and statically populated names.</t>
+  </si>
+  <si>
+    <t>• Worked on UI communicating with the database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,6 +146,22 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,8 +233,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -220,14 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -237,8 +254,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -294,7 +321,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -329,7 +356,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -506,7 +533,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,103 +543,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="9"/>
-    <col min="2" max="2" width="29.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="40.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="45" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+    <row r="2" spans="1:5">
+      <c r="A2" s="4">
         <v>42617</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" ht="65" customHeight="1">
+      <c r="A3" s="4">
         <f>A2+7</f>
         <v>42624</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:5" ht="69" customHeight="1">
+      <c r="A4" s="4">
         <f t="shared" ref="A4:A16" si="0">A3+7</f>
         <v>42631</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" ht="45">
+      <c r="A5" s="4">
         <f>A4+7</f>
         <v>42638</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+    <row r="6" spans="1:5" ht="48" customHeight="1">
+      <c r="A6" s="4">
         <f>A5+7</f>
         <v>42645</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
         <f t="shared" si="0"/>
         <v>42652</v>
       </c>
@@ -629,8 +656,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+    <row r="8" spans="1:5">
+      <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>42659</v>
       </c>
@@ -647,38 +674,62 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="4">
         <f t="shared" si="0"/>
         <v>42666</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>42673</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30">
+      <c r="A11" s="4">
         <f t="shared" si="0"/>
         <v>42680</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>42687</v>
       </c>
@@ -687,8 +738,8 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
         <f t="shared" si="0"/>
         <v>42694</v>
       </c>
@@ -697,8 +748,8 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+    <row r="14" spans="1:5">
+      <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>42701</v>
       </c>
@@ -707,8 +758,8 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+    <row r="15" spans="1:5">
+      <c r="A15" s="4">
         <f t="shared" si="0"/>
         <v>42708</v>
       </c>
@@ -717,8 +768,8 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
+    <row r="16" spans="1:5">
+      <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>42715</v>
       </c>
@@ -727,15 +778,15 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="10" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
@@ -743,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
@@ -759,5 +810,11 @@
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Weekly Logs till nov 22nd
</commit_message>
<xml_diff>
--- a/Weekly Logs.xlsx
+++ b/Weekly Logs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>• reached out to peers to form group</t>
   </si>
@@ -113,12 +113,64 @@
   </si>
   <si>
     <t>• Worked on UI communicating with the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>• learnt how to colour pages properly and worked on prototyping for the HomeViewController</t>
+  </si>
+  <si>
+    <t>• updated the SignInViewController to create Students as well as Users</t>
+  </si>
+  <si>
+    <t>• Finalized the App for presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Finalized the App for presentation and changed the UI </t>
+  </si>
+  <si>
+    <t>• Worked on the report
+• Worked on UI communicated with the database
+• Figured out how to code the transition of screens rather than using the Interface Builder</t>
+  </si>
+  <si>
+    <t>• Worked on UI (Home, Learn) Created prototypes and statically populated names.
+• Worked on making the UI dyanmic
+• Worked on populating courses in the search bar</t>
+  </si>
+  <si>
+    <t>• Worked on the database, made various functions. Also fixed errors</t>
+  </si>
+  <si>
+    <t>• Worked on UI (SignIn, Teach, Settings)
+• Worked on making the UI dyanmic
+• Worked on populating courses in the search bar</t>
+  </si>
+  <si>
+    <t>• Worked on UI (SignIn, Teach, Settings)
+• Sign in, sign up all works with databases , fixed navigation bars, got global variables to work</t>
+  </si>
+  <si>
+    <t>• Worked on UI communicated with the database
+• Figured out how to code the transition of screens rather than using the Interface Builder</t>
+  </si>
+  <si>
+    <t>• Worked on UI (Home, Learn)
+• Worked on making the UI dyanmic
+• Worked on populating courses in the search bar</t>
+  </si>
+  <si>
+    <t>• Discusses the things remaining to work on</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -167,12 +219,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -233,26 +291,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -262,10 +330,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,7 +633,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,75 +641,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="10.83203125" style="16"/>
     <col min="2" max="2" width="40.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="45" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4">
+      <c r="A2" s="16">
         <v>42617</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="65" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="16">
         <f>A2+7</f>
         <v>42624</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="69" customHeight="1">
-      <c r="A4" s="4">
-        <f t="shared" ref="A4:A16" si="0">A3+7</f>
+      <c r="A4" s="16">
+        <f t="shared" ref="A4:A11" si="0">A3+7</f>
         <v>42631</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="45">
-      <c r="A5" s="4">
+      <c r="A5" s="16">
         <f>A4+7</f>
         <v>42638</v>
       </c>
@@ -627,19 +727,19 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" customHeight="1">
-      <c r="A6" s="4">
+      <c r="A6" s="16">
         <f>A5+7</f>
         <v>42645</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4">
+      <c r="A7" s="16">
         <f t="shared" si="0"/>
         <v>42652</v>
       </c>
@@ -657,7 +757,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="4">
+      <c r="A8" s="16">
         <f t="shared" si="0"/>
         <v>42659</v>
       </c>
@@ -675,7 +775,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="4">
+      <c r="A9" s="16">
         <f t="shared" si="0"/>
         <v>42666</v>
       </c>
@@ -693,7 +793,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="4">
+      <c r="A10" s="16">
         <f t="shared" si="0"/>
         <v>42673</v>
       </c>
@@ -711,7 +811,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="4">
+      <c r="A11" s="16">
         <f t="shared" si="0"/>
         <v>42680</v>
       </c>
@@ -728,77 +828,147 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4">
-        <f t="shared" si="0"/>
+    <row r="12" spans="1:5" ht="60">
+      <c r="A12" s="16">
+        <v>42686</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60">
+      <c r="A13" s="16">
         <v>42687</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4">
-        <f t="shared" si="0"/>
-        <v>42694</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4">
-        <f t="shared" si="0"/>
-        <v>42701</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60">
+      <c r="A14" s="16">
+        <v>42688</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="4">
-        <f t="shared" si="0"/>
-        <v>42708</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="4">
-        <f t="shared" si="0"/>
-        <v>42715</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="B19" s="6" t="s">
+      <c r="A15" s="16">
+        <v>42690</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="16">
+        <v>42691</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45">
+      <c r="A17" s="16">
+        <v>42693</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="18" customFormat="1">
+      <c r="A18" s="17">
+        <v>42696</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="2" t="s">
+    <row r="27" spans="1:5">
+      <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
-      <c r="B21" s="2" t="s">
+    <row r="28" spans="1:5">
+      <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>